<commit_message>
ADD new trade status to clients
</commit_message>
<xml_diff>
--- a/worksheets/clients.xlsx
+++ b/worksheets/clients.xlsx
@@ -47,7 +47,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Status deve ser um dos seguintes tipos: Lead, Prospect, Cliente</t>
+          <t xml:space="preserve">Status deve ser um dos seguintes tipos: Lead, Prospect, Cliente, Ex Cliente, Lead com Proposta, Lead Inativo, Recusado, Restrito</t>
         </r>
       </text>
     </comment>
@@ -416,11 +416,11 @@
   </sheetPr>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V10" activeCellId="0" sqref="V10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.17"/>

</xml_diff>

<commit_message>
ALTE clients ADD seller FK
</commit_message>
<xml_diff>
--- a/worksheets/clients.xlsx
+++ b/worksheets/clients.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -134,6 +134,9 @@
     <t xml:space="preserve">filial</t>
   </si>
   <si>
+    <t xml:space="preserve">vendedor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Exemplo 1</t>
   </si>
   <si>
@@ -189,6 +192,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nome fantasia da filial ou vazio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome do vendedor igual ao do cadastro de vendedores</t>
   </si>
   <si>
     <t xml:space="preserve">Exemplo 2</t>
@@ -414,13 +420,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V7" activeCellId="0" sqref="V7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.17"/>
@@ -437,6 +443,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="21.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="27.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="47.76"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,132 +510,138 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S2" s="0" t="n">
         <v>100</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S3" s="5" t="n">
         <v>0</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ALTER import client worksheet add funnel porperties
</commit_message>
<xml_diff>
--- a/worksheets/clients.xlsx
+++ b/worksheets/clients.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -38,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -47,11 +47,11 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Status deve ser um dos seguintes tipos: Lead, Prospect, Cliente, Ex Cliente, Lead com Proposta, Lead Inativo, Recusado, Restrito</t>
+          <t xml:space="preserve">Status deve ser um dos seguintes tipos: Prospect, Prospect com Interesse, Lead, Lead com Proposta, Lead Inativo, Contato Realizado, Vistoria Marcada, Aguardando Orçamento, Orçamento Enviado, Assembléia Marcada, Negociação, Venda Realizada, Cliente, Ex Cliente, Recusado ou Restrito</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -64,16 +64,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="AA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Valores aceitos: Contrato em Confecção, Contrato Assinado, Aguardando PG, Entrada PG, Aguardando Vistoria para Obra, Início de Obra, Obra em andamento, Obra Finalizada, Obra Entregue ou Início de Leitura</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
   <si>
+    <t xml:space="preserve">vendedor</t>
+  </si>
+  <si>
     <t xml:space="preserve">cpf_cnpj</t>
   </si>
   <si>
@@ -89,6 +105,9 @@
     <t xml:space="preserve">contato</t>
   </si>
   <si>
+    <t xml:space="preserve">funcao_contato</t>
+  </si>
+  <si>
     <t xml:space="preserve">email</t>
   </si>
   <si>
@@ -125,21 +144,36 @@
     <t xml:space="preserve">empresa</t>
   </si>
   <si>
+    <t xml:space="preserve">valor_por_apartamento</t>
+  </si>
+  <si>
     <t xml:space="preserve">apartamentos</t>
   </si>
   <si>
+    <t xml:space="preserve">valor_total</t>
+  </si>
+  <si>
     <t xml:space="preserve">observacoes</t>
   </si>
   <si>
     <t xml:space="preserve">filial</t>
   </si>
   <si>
-    <t xml:space="preserve">vendedor</t>
+    <t xml:space="preserve">assembleia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status_venda_realizada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motivo_recusa</t>
   </si>
   <si>
     <t xml:space="preserve">Exemplo 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Cardoso</t>
+  </si>
+  <si>
     <t xml:space="preserve">000.000.000-00</t>
   </si>
   <si>
@@ -155,6 +189,9 @@
     <t xml:space="preserve">Dados do contato</t>
   </si>
   <si>
+    <t xml:space="preserve">Síndico</t>
+  </si>
+  <si>
     <t xml:space="preserve">fulano@gmail.com</t>
   </si>
   <si>
@@ -191,10 +228,13 @@
     <t xml:space="preserve">qualquer informação útil</t>
   </si>
   <si>
-    <t xml:space="preserve">Nome fantasia da filial ou vazio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nome do vendedor igual ao do cadastro de vendedores</t>
+    <t xml:space="preserve">Acqua X do Brasil - ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/12/2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blá blá blá pode ser nulo, editar somente quando o status for recusado</t>
   </si>
   <si>
     <t xml:space="preserve">Exemplo 2</t>
@@ -212,20 +252,30 @@
     <t xml:space="preserve">oHub</t>
   </si>
   <si>
+    <t xml:space="preserve">Gerente</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vitória</t>
   </si>
   <si>
     <t xml:space="preserve">ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acqua X do Brasil - RJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contrato em Confecção</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -258,6 +308,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -318,7 +376,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,7 +393,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,40 +486,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V7" activeCellId="0" sqref="V7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="17.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="12.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="21.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="27.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="47.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="18.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="24.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="0" width="21.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="27.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="60.44"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -462,34 +530,34 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -504,150 +572,198 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="W2" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="0" t="s">
+      <c r="H3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="J3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="K3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="T2" s="0" t="s">
+      <c r="L3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="M3" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="0" t="s">
+      <c r="N3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="P3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="Q3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="T3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="5" t="n">
+      <c r="U3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="5" t="s">
+      <c r="V3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>39</v>
+      <c r="Y3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId2" display="fulano@gmail.com"/>
-    <hyperlink ref="G3" r:id="rId3" display="fulano@gmail.com"/>
+    <hyperlink ref="I2" r:id="rId2" display="fulano@gmail.com"/>
+    <hyperlink ref="I3" r:id="rId3" display="fulano@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>